<commit_message>
ADD some new TS for calc
</commit_message>
<xml_diff>
--- a/test_scenarios_calc/test_web_calc_v3.xlsx
+++ b/test_scenarios_calc/test_web_calc_v3.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="172">
   <si>
     <t>Сценарии тестирования веб-калькулятора деления</t>
   </si>
@@ -484,13 +484,55 @@
     <t>Проверка корректности работы API при обращении из различных браузеров. Chrome</t>
   </si>
   <si>
-    <t>Успешное прохождение теста</t>
-  </si>
-  <si>
     <t>Проверка корректности работы API при обращении из различных браузеров. Firefox</t>
   </si>
   <si>
     <t>Проверка корректности работы API при обращении из различных браузеров. Другие поддерживаемые браузеры</t>
+  </si>
+  <si>
+    <t>Успешное прохождение тестов</t>
+  </si>
+  <si>
+    <t>TS13</t>
+  </si>
+  <si>
+    <t>TС13.01</t>
+  </si>
+  <si>
+    <t>Очистка полей ввода</t>
+  </si>
+  <si>
+    <t>Ввод данных в числитель</t>
+  </si>
+  <si>
+    <t>TС13.02</t>
+  </si>
+  <si>
+    <t>Проверка что пользователь может очищать введенные данные в числителе</t>
+  </si>
+  <si>
+    <t>Проверка что пользователь может очищать введенные данные в знаменателе</t>
+  </si>
+  <si>
+    <t>Данные удалены в поле ввода</t>
+  </si>
+  <si>
+    <t>TS14</t>
+  </si>
+  <si>
+    <t>Кешируемость</t>
+  </si>
+  <si>
+    <t>TС14.01</t>
+  </si>
+  <si>
+    <t>Проверка обновления результата при вводе других данных</t>
+  </si>
+  <si>
+    <t>Результат обновлен</t>
+  </si>
+  <si>
+    <t>Повторное вычисление с новыми данными</t>
   </si>
 </sst>
 </file>
@@ -965,7 +1007,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1075,6 +1117,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
@@ -1379,8 +1422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2156,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="55"/>
@@ -2122,76 +2165,90 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G44" s="43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="55" t="s">
+        <v>166</v>
+      </c>
+      <c r="B44" s="55" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" s="55" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" s="55" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" s="55" t="s">
+        <v>170</v>
+      </c>
+      <c r="G44" s="52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
-      <c r="D45" s="3" t="s">
-        <v>156</v>
-      </c>
+      <c r="D45" s="3"/>
       <c r="E45" s="3"/>
-      <c r="F45" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G45" s="43" t="s">
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G46" s="61" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="G46" s="43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>155</v>
+      </c>
       <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F47" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G47" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2200,23 +2257,47 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G50" s="43" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
+      <c r="C51" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="G51" s="43" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="52" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3"/>

</xml_diff>